<commit_message>
import updated impact factor files and try processing
</commit_message>
<xml_diff>
--- a/oregon_deq/source_data/mrs_x_deq_xwalk.xlsx
+++ b/oregon_deq/source_data/mrs_x_deq_xwalk.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="64">
   <si>
     <t>material</t>
   </si>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>Carpeting-used</t>
+  </si>
+  <si>
+    <t>Nonrecyclables</t>
+  </si>
+  <si>
+    <t>RigidPlastic</t>
+  </si>
+  <si>
+    <t>YardDebris</t>
   </si>
 </sst>
 </file>
@@ -1009,11 +1018,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J66"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,9 +1031,11 @@
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1049,8 +1060,14 @@
       <c r="J1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1076,7 +1093,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1096,7 +1113,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1122,7 +1139,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1142,7 +1159,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1168,7 +1185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1194,7 +1211,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1208,7 +1225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1221,67 +1238,61 @@
       <c r="G9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
         <v>45</v>
       </c>
-      <c r="G10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
       </c>
-      <c r="F12" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
         <v>44</v>
@@ -1296,18 +1307,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I14" t="s">
         <v>46</v>
@@ -1316,18 +1327,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="I15" t="s">
         <v>59</v>
@@ -1336,18 +1347,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I16" t="s">
         <v>59</v>
@@ -1358,10 +1369,16 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
       </c>
       <c r="F17" t="s">
         <v>42</v>
@@ -1381,7 +1398,13 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
       </c>
       <c r="F18" t="s">
         <v>41</v>
@@ -1401,19 +1424,19 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
       </c>
       <c r="F19" t="s">
         <v>41</v>
       </c>
       <c r="G19" t="s">
         <v>20</v>
-      </c>
-      <c r="I19" t="s">
-        <v>45</v>
-      </c>
-      <c r="J19" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1421,7 +1444,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
         <v>40</v>
@@ -1429,25 +1452,13 @@
       <c r="G20" t="s">
         <v>20</v>
       </c>
-      <c r="I20" t="s">
-        <v>45</v>
-      </c>
-      <c r="J20" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F21" t="s">
         <v>39</v>
@@ -1464,16 +1475,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F22" t="s">
         <v>38</v>
@@ -1490,16 +1495,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F23" t="s">
         <v>37</v>
@@ -1510,15 +1509,9 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" t="s">
         <v>6</v>
       </c>
       <c r="F24" t="s">
@@ -1530,15 +1523,9 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" t="s">
         <v>3</v>
       </c>
       <c r="I25" t="s">
@@ -1550,33 +1537,27 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
         <v>3</v>
@@ -1590,13 +1571,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
         <v>20</v>
@@ -1616,16 +1597,16 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F29" t="s">
         <v>34</v>
@@ -1642,16 +1623,16 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F30" t="s">
         <v>33</v>
@@ -1667,10 +1648,16 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
         <v>20</v>
       </c>
       <c r="I31" t="s">
@@ -1681,6 +1668,18 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
       <c r="F32" t="s">
         <v>31</v>
       </c>
@@ -1694,7 +1693,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
       <c r="I33" t="s">
         <v>40</v>
       </c>
@@ -1702,7 +1713,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
       <c r="F34" t="s">
         <v>29</v>
       </c>
@@ -1716,7 +1739,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
       <c r="F35" t="s">
         <v>29</v>
       </c>
@@ -1730,7 +1765,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>20</v>
+      </c>
       <c r="F36" t="s">
         <v>28</v>
       </c>
@@ -1744,7 +1791,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
       <c r="F37" t="s">
         <v>28</v>
       </c>
@@ -1758,7 +1817,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" t="s">
+        <v>20</v>
+      </c>
       <c r="I38" t="s">
         <v>37</v>
       </c>
@@ -1766,7 +1837,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
       <c r="F39" t="s">
         <v>26</v>
       </c>
@@ -1774,7 +1851,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" t="s">
+        <v>22</v>
+      </c>
       <c r="F40" t="s">
         <v>26</v>
       </c>
@@ -1782,7 +1871,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" t="s">
+        <v>23</v>
+      </c>
       <c r="F41" t="s">
         <v>25</v>
       </c>
@@ -1790,7 +1891,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
       <c r="F42" t="s">
         <v>25</v>
       </c>
@@ -1798,7 +1911,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>24</v>
       </c>
@@ -1812,7 +1925,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
         <v>24</v>
       </c>
@@ -1826,41 +1939,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
         <v>24</v>
       </c>
       <c r="G45" t="s">
         <v>20</v>
       </c>
-      <c r="I45" t="s">
-        <v>32</v>
-      </c>
-      <c r="J45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F46" t="s">
-        <v>21</v>
-      </c>
-      <c r="G46" t="s">
-        <v>23</v>
-      </c>
-      <c r="I46" t="s">
-        <v>32</v>
-      </c>
-      <c r="J46" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F47" t="s">
-        <v>21</v>
-      </c>
-      <c r="G47" t="s">
-        <v>22</v>
-      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I47" t="s">
         <v>31</v>
       </c>
@@ -1868,7 +1955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
         <v>21</v>
       </c>
@@ -1975,22 +2062,6 @@
         <v>24</v>
       </c>
       <c r="J62" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I63" t="s">
-        <v>21</v>
-      </c>
-      <c r="J63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I64" t="s">
-        <v>21</v>
-      </c>
-      <c r="J64" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
revise arr code to include custom miles
</commit_message>
<xml_diff>
--- a/oregon_deq/source_data/mrs_x_deq_xwalk.xlsx
+++ b/oregon_deq/source_data/mrs_x_deq_xwalk.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="64">
   <si>
     <t>material</t>
   </si>
@@ -1021,8 +1021,8 @@
   <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I65" sqref="I65"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,15 +1275,15 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
         <v>45</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1292,7 +1292,13 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
       </c>
       <c r="F13" t="s">
         <v>44</v>
@@ -1318,7 +1324,7 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="I14" t="s">
         <v>46</v>
@@ -1332,13 +1338,13 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I15" t="s">
         <v>59</v>
@@ -1352,13 +1358,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="I16" t="s">
         <v>59</v>
@@ -1369,13 +1375,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="D17" t="s">
         <v>3</v>
@@ -1398,13 +1404,13 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
         <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F18" t="s">
         <v>41</v>
@@ -1424,13 +1430,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
         <v>41</v>
@@ -1444,7 +1444,7 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F20" t="s">
         <v>40</v>
@@ -1458,7 +1458,7 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F21" t="s">
         <v>39</v>
@@ -1478,7 +1478,7 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F22" t="s">
         <v>38</v>
@@ -1495,10 +1495,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F23" t="s">
         <v>37</v>
@@ -1512,7 +1512,7 @@
         <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F24" t="s">
         <v>37</v>
@@ -1523,10 +1523,16 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
       </c>
       <c r="I25" t="s">
         <v>43</v>
@@ -1540,13 +1546,13 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
         <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1554,13 +1560,13 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
         <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I27" t="s">
         <v>57</v>
@@ -1571,16 +1577,16 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F28" t="s">
         <v>34</v>
@@ -1600,13 +1606,13 @@
         <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="F29" t="s">
         <v>34</v>
@@ -1626,13 +1632,13 @@
         <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F30" t="s">
         <v>33</v>
@@ -1649,16 +1655,16 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D31" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I31" t="s">
         <v>41</v>
@@ -1672,13 +1678,13 @@
         <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
         <v>32</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F32" t="s">
         <v>31</v>
@@ -1698,13 +1704,13 @@
         <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I33" t="s">
         <v>40</v>
@@ -1715,16 +1721,16 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F34" t="s">
         <v>29</v>
@@ -1744,13 +1750,13 @@
         <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
         <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F35" t="s">
         <v>29</v>
@@ -1767,16 +1773,16 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F36" t="s">
         <v>28</v>
@@ -1796,13 +1802,13 @@
         <v>19</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C37" t="s">
         <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F37" t="s">
         <v>28</v>
@@ -1819,16 +1825,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="I38" t="s">
         <v>37</v>
@@ -1842,7 +1842,13 @@
         <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s">
+        <v>22</v>
       </c>
       <c r="F39" t="s">
         <v>26</v>
@@ -1856,13 +1862,13 @@
         <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C40" t="s">
         <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F40" t="s">
         <v>26</v>
@@ -1876,13 +1882,13 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
         <v>21</v>
       </c>
       <c r="D41" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F41" t="s">
         <v>25</v>
@@ -1892,18 +1898,6 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" t="s">
-        <v>3</v>
-      </c>
       <c r="F42" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
fix (in a temporary way) missing tons in dispose_all
</commit_message>
<xml_diff>
--- a/oregon_deq/source_data/mrs_x_deq_xwalk.xlsx
+++ b/oregon_deq/source_data/mrs_x_deq_xwalk.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deqhq1\swrshare\!PROGRAMS-SOLID-WASTE-(PSW)\LCA\Projects\IMFO\waste-impact-calculator\oregon_deq\source_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\deqhq1\SWRSHARE\!PROGRAMS-SOLID-WASTE-(PSW)\LCA\Projects\IMFO\waste-impact-calculator\oregon_deq\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="65">
   <si>
     <t>material</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>YardDebris</t>
+  </si>
+  <si>
+    <t>Wood</t>
   </si>
 </sst>
 </file>
@@ -1018,11 +1021,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M66"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:D12"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1038,7 @@
     <col min="13" max="13" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1067,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1132,14 +1135,20 @@
       <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>2</v>
       </c>
-      <c r="J4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1159,7 +1168,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1185,7 +1194,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1211,7 +1220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1225,7 +1234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1245,7 +1254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1259,7 +1268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1273,7 +1282,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1287,7 +1296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1313,7 +1322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1333,7 +1342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1353,7 +1362,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1392,12 +1401,6 @@
       <c r="G17" t="s">
         <v>20</v>
       </c>
-      <c r="I17" t="s">
-        <v>58</v>
-      </c>
-      <c r="J17" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1418,12 +1421,6 @@
       <c r="G18" t="s">
         <v>22</v>
       </c>
-      <c r="I18" t="s">
-        <v>58</v>
-      </c>
-      <c r="J18" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1500,6 +1497,12 @@
       <c r="B23" t="s">
         <v>6</v>
       </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
       <c r="F23" t="s">
         <v>37</v>
       </c>
@@ -1514,6 +1517,12 @@
       <c r="B24" t="s">
         <v>3</v>
       </c>
+      <c r="C24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" t="s">
+        <v>3</v>
+      </c>
       <c r="F24" t="s">
         <v>37</v>
       </c>
@@ -1825,10 +1834,16 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" t="s">
+        <v>23</v>
       </c>
       <c r="I38" t="s">
         <v>37</v>
@@ -1839,13 +1854,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D39" t="s">
         <v>22</v>
@@ -1859,16 +1874,16 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F40" t="s">
         <v>26</v>
@@ -1879,16 +1894,16 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F41" t="s">
         <v>25</v>
@@ -1898,6 +1913,12 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>9</v>
+      </c>
       <c r="F42" t="s">
         <v>25</v>
       </c>
@@ -1906,11 +1927,17 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F43" t="s">
-        <v>24</v>
-      </c>
-      <c r="G43" t="s">
-        <v>23</v>
+      <c r="A43" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s">
+        <v>22</v>
       </c>
       <c r="I43" t="s">
         <v>34</v>
@@ -1920,11 +1947,23 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" t="s">
+        <v>23</v>
+      </c>
       <c r="F44" t="s">
         <v>24</v>
       </c>
       <c r="G44" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I44" t="s">
         <v>34</v>
@@ -1934,11 +1973,17 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F45" t="s">
-        <v>24</v>
-      </c>
-      <c r="G45" t="s">
-        <v>20</v>
+      <c r="A45" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -2054,9 +2099,6 @@
     <row r="62" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I62" t="s">
         <v>24</v>
-      </c>
-      <c r="J62" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="65" spans="9:10" x14ac:dyDescent="0.25">

</xml_diff>